<commit_message>
Python (Statgrad 2025-1) V-2
</commit_message>
<xml_diff>
--- a/python/EGE/Статград/1-2025/Доп/18.xlsx
+++ b/python/EGE/Статград/1-2025/Доп/18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ЕГЭ\2025\ТР1\Файлы 2025 ТР1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snser\OneDrive\Документы\GitHub\Python\python\EGE\Статград\1-2025\Доп\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461DBD8E-97CB-4B59-9FEF-E433A2861039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E173486-ACDA-466B-B156-62B8291E8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="18" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,6 +59,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -172,6 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -476,19 +484,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:U21"/>
+  <dimension ref="B1:AP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="21" width="4.6328125" customWidth="1"/>
+    <col min="2" max="21" width="4.5703125" customWidth="1"/>
+    <col min="23" max="42" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>15</v>
       </c>
@@ -549,8 +558,88 @@
       <c r="U2" s="4">
         <v>21</v>
       </c>
+      <c r="W2" s="1">
+        <f>B2</f>
+        <v>15</v>
+      </c>
+      <c r="X2" s="2">
+        <f>W2+C2</f>
+        <v>39</v>
+      </c>
+      <c r="Y2" s="2">
+        <f t="shared" ref="Y2:AP2" si="0">X2+D2</f>
+        <v>60</v>
+      </c>
+      <c r="Z2" s="2">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="AA2" s="2">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="AB2" s="2">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="AC2" s="2">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="AD2" s="2">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="AE2" s="2">
+        <f t="shared" si="0"/>
+        <v>206</v>
+      </c>
+      <c r="AF2" s="2">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="AG2" s="2">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="AH2" s="2">
+        <f t="shared" si="0"/>
+        <v>316</v>
+      </c>
+      <c r="AI2" s="2">
+        <f t="shared" si="0"/>
+        <v>386</v>
+      </c>
+      <c r="AJ2" s="2">
+        <f t="shared" si="0"/>
+        <v>434</v>
+      </c>
+      <c r="AK2" s="2">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="AL2" s="2">
+        <f t="shared" si="0"/>
+        <v>453</v>
+      </c>
+      <c r="AM2" s="2">
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+      <c r="AN2" s="2">
+        <f t="shared" si="0"/>
+        <v>482</v>
+      </c>
+      <c r="AO2" s="2">
+        <f t="shared" si="0"/>
+        <v>528</v>
+      </c>
+      <c r="AP2" s="2">
+        <f t="shared" si="0"/>
+        <v>549</v>
+      </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>75</v>
       </c>
@@ -611,8 +700,88 @@
       <c r="U3" s="7">
         <v>80</v>
       </c>
+      <c r="W3" s="5">
+        <f>W2+B3</f>
+        <v>90</v>
+      </c>
+      <c r="X3" s="6">
+        <f>MIN(W3,X2)+C3</f>
+        <v>94</v>
+      </c>
+      <c r="Y3" s="6">
+        <f t="shared" ref="Y3:AP3" si="1">MIN(X3,Y2)+D3</f>
+        <v>107</v>
+      </c>
+      <c r="Z3" s="6">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="AA3" s="6">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="AB3" s="6">
+        <f t="shared" si="1"/>
+        <v>181</v>
+      </c>
+      <c r="AC3" s="6">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+      <c r="AD3" s="6">
+        <f t="shared" si="1"/>
+        <v>246</v>
+      </c>
+      <c r="AE3" s="6">
+        <f t="shared" si="1"/>
+        <v>304</v>
+      </c>
+      <c r="AF3" s="6">
+        <f t="shared" si="1"/>
+        <v>314</v>
+      </c>
+      <c r="AG3" s="6">
+        <f t="shared" si="1"/>
+        <v>295</v>
+      </c>
+      <c r="AH3" s="6">
+        <f t="shared" si="1"/>
+        <v>356</v>
+      </c>
+      <c r="AI3" s="6">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+      <c r="AJ3" s="6">
+        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="AK3" s="6">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="AL3" s="6">
+        <f t="shared" si="1"/>
+        <v>489</v>
+      </c>
+      <c r="AM3" s="6">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="AN3" s="6">
+        <f t="shared" si="1"/>
+        <v>514</v>
+      </c>
+      <c r="AO3" s="6">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+      <c r="AP3" s="6">
+        <f t="shared" si="1"/>
+        <v>629</v>
+      </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>59</v>
       </c>
@@ -673,8 +842,87 @@
       <c r="U4" s="7">
         <v>41</v>
       </c>
+      <c r="W4" s="5">
+        <f t="shared" ref="W4:W21" si="2">W3+B4</f>
+        <v>149</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" ref="X4:X21" si="3">MIN(W4,X3)+C4</f>
+        <v>175</v>
+      </c>
+      <c r="Y4" s="6">
+        <f t="shared" ref="Y4:Y21" si="4">MIN(X4,Y3)+D4</f>
+        <v>140</v>
+      </c>
+      <c r="Z4" s="6">
+        <f t="shared" ref="Z4:Z21" si="5">MIN(Y4,Z3)+E4</f>
+        <v>132</v>
+      </c>
+      <c r="AA4" s="6">
+        <f t="shared" ref="AA4:AA21" si="6">MIN(Z4,AA3)+F4</f>
+        <v>180</v>
+      </c>
+      <c r="AB4" s="6">
+        <f t="shared" ref="AB4:AB21" si="7">MIN(AA4,AB3)+G4</f>
+        <v>185</v>
+      </c>
+      <c r="AC4" s="6">
+        <f t="shared" ref="AC4:AC21" si="8">MIN(AB4,AC3)+H4</f>
+        <v>247</v>
+      </c>
+      <c r="AD4" s="6">
+        <f t="shared" ref="AD4:AD21" si="9">MIN(AC4,AD3)+I4</f>
+        <v>288</v>
+      </c>
+      <c r="AE4" s="6">
+        <f t="shared" ref="AE4:AE21" si="10">MIN(AD4,AE3)+J4</f>
+        <v>343</v>
+      </c>
+      <c r="AF4" s="6">
+        <f t="shared" ref="AF4:AF21" si="11">MIN(AE4,AF3)+K4</f>
+        <v>407</v>
+      </c>
+      <c r="AG4" s="6">
+        <f t="shared" ref="AG4:AG21" si="12">MIN(AF4,AG3)+L4</f>
+        <v>338</v>
+      </c>
+      <c r="AH4" s="6">
+        <f t="shared" ref="AH4:AH21" si="13">MIN(AG4,AH3)+M4</f>
+        <v>354</v>
+      </c>
+      <c r="AI4" s="6">
+        <f t="shared" ref="AI4:AI21" si="14">MIN(AH4,AI3)+N4</f>
+        <v>399</v>
+      </c>
+      <c r="AJ4" s="6">
+        <f t="shared" ref="AJ4:AJ21" si="15">MIN(AI4,AJ3)+O4</f>
+        <v>496</v>
+      </c>
+      <c r="AK4" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AL4">
+        <f t="shared" ref="AL4:AL21" si="16">MIN(AK4,AL3)+Q4</f>
+        <v>514</v>
+      </c>
+      <c r="AM4" s="6">
+        <f t="shared" ref="AM4:AM21" si="17">MIN(AL4,AM3)+R4</f>
+        <v>549</v>
+      </c>
+      <c r="AN4" s="6">
+        <f t="shared" ref="AN4:AN21" si="18">MIN(AM4,AN3)+S4</f>
+        <v>611</v>
+      </c>
+      <c r="AO4" s="6">
+        <f t="shared" ref="AO4:AO21" si="19">MIN(AN4,AO3)+T4</f>
+        <v>643</v>
+      </c>
+      <c r="AP4" s="7">
+        <f t="shared" ref="AP4:AP21" si="20">MIN(AO4,AP3)+U4</f>
+        <v>670</v>
+      </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>85</v>
       </c>
@@ -735,8 +983,83 @@
       <c r="U5" s="7">
         <v>82</v>
       </c>
+      <c r="W5" s="5">
+        <f t="shared" si="2"/>
+        <v>234</v>
+      </c>
+      <c r="X5" s="6">
+        <f t="shared" si="3"/>
+        <v>227</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+      <c r="Z5" s="6">
+        <f t="shared" si="5"/>
+        <v>215</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AB5" s="6">
+        <f t="shared" si="7"/>
+        <v>211</v>
+      </c>
+      <c r="AC5" s="6">
+        <f t="shared" si="8"/>
+        <v>219</v>
+      </c>
+      <c r="AD5" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AE5" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AF5" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AG5" s="6">
+        <f t="shared" si="12"/>
+        <v>435</v>
+      </c>
+      <c r="AH5" s="6">
+        <f t="shared" si="13"/>
+        <v>375</v>
+      </c>
+      <c r="AI5" s="6">
+        <f t="shared" si="14"/>
+        <v>408</v>
+      </c>
+      <c r="AJ5" s="6">
+        <f t="shared" si="15"/>
+        <v>489</v>
+      </c>
+      <c r="AK5" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="16"/>
+        <v>527</v>
+      </c>
+      <c r="AM5" s="6">
+        <f t="shared" si="17"/>
+        <v>597</v>
+      </c>
+      <c r="AN5" s="6">
+        <f t="shared" si="18"/>
+        <v>689</v>
+      </c>
+      <c r="AO5" s="6">
+        <f t="shared" si="19"/>
+        <v>720</v>
+      </c>
+      <c r="AP5" s="7">
+        <f t="shared" si="20"/>
+        <v>752</v>
+      </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>12</v>
       </c>
@@ -797,8 +1120,85 @@
       <c r="U6" s="7">
         <v>22</v>
       </c>
+      <c r="W6" s="5">
+        <f t="shared" si="2"/>
+        <v>246</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="3"/>
+        <v>259</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="4"/>
+        <v>247</v>
+      </c>
+      <c r="Z6" s="6">
+        <f t="shared" si="5"/>
+        <v>221</v>
+      </c>
+      <c r="AA6" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AB6" s="6">
+        <f t="shared" si="7"/>
+        <v>269</v>
+      </c>
+      <c r="AC6" s="6">
+        <f t="shared" si="8"/>
+        <v>284</v>
+      </c>
+      <c r="AD6" s="6">
+        <f t="shared" si="9"/>
+        <v>374</v>
+      </c>
+      <c r="AE6" s="6">
+        <f t="shared" si="10"/>
+        <v>425</v>
+      </c>
+      <c r="AF6" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AG6" s="6">
+        <f t="shared" si="12"/>
+        <v>437</v>
+      </c>
+      <c r="AH6" s="6">
+        <f t="shared" si="13"/>
+        <v>385</v>
+      </c>
+      <c r="AI6" s="6">
+        <f t="shared" si="14"/>
+        <v>468</v>
+      </c>
+      <c r="AJ6" s="6">
+        <f t="shared" si="15"/>
+        <v>544</v>
+      </c>
+      <c r="AK6" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AL6">
+        <f t="shared" si="16"/>
+        <v>618</v>
+      </c>
+      <c r="AM6" s="6">
+        <f t="shared" si="17"/>
+        <v>649</v>
+      </c>
+      <c r="AN6" s="6">
+        <f t="shared" si="18"/>
+        <v>696</v>
+      </c>
+      <c r="AO6" s="6">
+        <f t="shared" si="19"/>
+        <v>790</v>
+      </c>
+      <c r="AP6" s="7">
+        <f t="shared" si="20"/>
+        <v>774</v>
+      </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>90</v>
       </c>
@@ -859,8 +1259,85 @@
       <c r="U7" s="7">
         <v>53</v>
       </c>
+      <c r="W7" s="5">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="3"/>
+        <v>263</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="4"/>
+        <v>264</v>
+      </c>
+      <c r="Z7" s="6">
+        <f t="shared" si="5"/>
+        <v>316</v>
+      </c>
+      <c r="AA7" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AB7" s="6">
+        <f t="shared" si="7"/>
+        <v>342</v>
+      </c>
+      <c r="AC7" s="6">
+        <f t="shared" si="8"/>
+        <v>346</v>
+      </c>
+      <c r="AD7" s="6">
+        <f t="shared" si="9"/>
+        <v>443</v>
+      </c>
+      <c r="AE7" s="6">
+        <f t="shared" si="10"/>
+        <v>458</v>
+      </c>
+      <c r="AF7" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AG7" s="6">
+        <f t="shared" si="12"/>
+        <v>527</v>
+      </c>
+      <c r="AH7" s="6">
+        <f t="shared" si="13"/>
+        <v>444</v>
+      </c>
+      <c r="AI7" s="6">
+        <f t="shared" si="14"/>
+        <v>491</v>
+      </c>
+      <c r="AJ7" s="16">
+        <f t="shared" si="15"/>
+        <v>526</v>
+      </c>
+      <c r="AK7" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="16"/>
+        <v>710</v>
+      </c>
+      <c r="AM7" s="6">
+        <f t="shared" si="17"/>
+        <v>678</v>
+      </c>
+      <c r="AN7" s="6">
+        <f t="shared" si="18"/>
+        <v>703</v>
+      </c>
+      <c r="AO7" s="6">
+        <f t="shared" si="19"/>
+        <v>734</v>
+      </c>
+      <c r="AP7" s="7">
+        <f t="shared" si="20"/>
+        <v>787</v>
+      </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>53</v>
       </c>
@@ -921,8 +1398,82 @@
       <c r="U8" s="7">
         <v>2</v>
       </c>
+      <c r="W8" s="5">
+        <f t="shared" si="2"/>
+        <v>389</v>
+      </c>
+      <c r="X8" s="6">
+        <f t="shared" si="3"/>
+        <v>334</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" si="4"/>
+        <v>307</v>
+      </c>
+      <c r="Z8" s="16">
+        <f t="shared" si="5"/>
+        <v>391</v>
+      </c>
+      <c r="AA8" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AB8" s="6">
+        <f t="shared" si="7"/>
+        <v>392</v>
+      </c>
+      <c r="AC8" s="6">
+        <f t="shared" si="8"/>
+        <v>437</v>
+      </c>
+      <c r="AD8" s="6">
+        <f t="shared" si="9"/>
+        <v>472</v>
+      </c>
+      <c r="AE8" s="6">
+        <f t="shared" si="10"/>
+        <v>470</v>
+      </c>
+      <c r="AF8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AG8" s="6">
+        <f t="shared" si="12"/>
+        <v>558</v>
+      </c>
+      <c r="AH8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AI8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AJ8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AK8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" si="16"/>
+        <v>785</v>
+      </c>
+      <c r="AM8" s="6">
+        <f t="shared" si="17"/>
+        <v>687</v>
+      </c>
+      <c r="AN8" s="6">
+        <f t="shared" si="18"/>
+        <v>749</v>
+      </c>
+      <c r="AO8" s="6">
+        <f t="shared" si="19"/>
+        <v>823</v>
+      </c>
+      <c r="AP8" s="7">
+        <f t="shared" si="20"/>
+        <v>789</v>
+      </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>34</v>
       </c>
@@ -983,8 +1534,84 @@
       <c r="U9" s="7">
         <v>48</v>
       </c>
+      <c r="W9" s="5">
+        <f t="shared" si="2"/>
+        <v>423</v>
+      </c>
+      <c r="X9" s="6">
+        <f t="shared" si="3"/>
+        <v>341</v>
+      </c>
+      <c r="Y9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="Z9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AA9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="AB9" s="6">
+        <f t="shared" si="7"/>
+        <v>407</v>
+      </c>
+      <c r="AC9" s="6">
+        <f t="shared" si="8"/>
+        <v>439</v>
+      </c>
+      <c r="AD9" s="6">
+        <f t="shared" si="9"/>
+        <v>504</v>
+      </c>
+      <c r="AE9" s="6">
+        <f t="shared" si="10"/>
+        <v>491</v>
+      </c>
+      <c r="AF9" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="AG9" s="6">
+        <f t="shared" si="12"/>
+        <v>637</v>
+      </c>
+      <c r="AH9" s="6">
+        <f t="shared" si="13"/>
+        <v>655</v>
+      </c>
+      <c r="AI9" s="6">
+        <f t="shared" si="14"/>
+        <v>710</v>
+      </c>
+      <c r="AJ9" s="6">
+        <f t="shared" si="15"/>
+        <v>809</v>
+      </c>
+      <c r="AK9" s="6">
+        <f t="shared" ref="AK4:AK21" si="21">MIN(AJ9,AK8)+P9</f>
+        <v>810</v>
+      </c>
+      <c r="AL9">
+        <f t="shared" si="16"/>
+        <v>796</v>
+      </c>
+      <c r="AM9" s="6">
+        <f t="shared" si="17"/>
+        <v>774</v>
+      </c>
+      <c r="AN9" s="6">
+        <f t="shared" si="18"/>
+        <v>819</v>
+      </c>
+      <c r="AO9" s="6">
+        <f t="shared" si="19"/>
+        <v>898</v>
+      </c>
+      <c r="AP9" s="7">
+        <f t="shared" si="20"/>
+        <v>837</v>
+      </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>45</v>
       </c>
@@ -1045,8 +1672,85 @@
       <c r="U10" s="7">
         <v>18</v>
       </c>
+      <c r="W10" s="5">
+        <f t="shared" si="2"/>
+        <v>468</v>
+      </c>
+      <c r="X10" s="6">
+        <f t="shared" si="3"/>
+        <v>361</v>
+      </c>
+      <c r="Y10" s="6">
+        <f t="shared" si="4"/>
+        <v>367</v>
+      </c>
+      <c r="Z10" s="6">
+        <f t="shared" si="5"/>
+        <v>459</v>
+      </c>
+      <c r="AA10" s="6">
+        <f t="shared" si="6"/>
+        <v>474</v>
+      </c>
+      <c r="AB10" s="6">
+        <f t="shared" si="7"/>
+        <v>495</v>
+      </c>
+      <c r="AC10" s="6">
+        <f t="shared" si="8"/>
+        <v>489</v>
+      </c>
+      <c r="AD10" s="6">
+        <f t="shared" si="9"/>
+        <v>506</v>
+      </c>
+      <c r="AE10" s="6">
+        <f t="shared" si="10"/>
+        <v>512</v>
+      </c>
+      <c r="AF10" s="6">
+        <f t="shared" si="11"/>
+        <v>518</v>
+      </c>
+      <c r="AG10" s="6">
+        <f t="shared" si="12"/>
+        <v>564</v>
+      </c>
+      <c r="AH10" s="6">
+        <f t="shared" si="13"/>
+        <v>662</v>
+      </c>
+      <c r="AI10" s="6">
+        <f t="shared" si="14"/>
+        <v>737</v>
+      </c>
+      <c r="AJ10" s="6">
+        <f t="shared" si="15"/>
+        <v>769</v>
+      </c>
+      <c r="AK10" s="6">
+        <f t="shared" si="21"/>
+        <v>849</v>
+      </c>
+      <c r="AL10">
+        <f t="shared" si="16"/>
+        <v>848</v>
+      </c>
+      <c r="AM10" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AN10" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AO10" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP10" s="7">
+        <f t="shared" si="20"/>
+        <v>855</v>
+      </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>68</v>
       </c>
@@ -1107,8 +1811,87 @@
       <c r="U11" s="7">
         <v>94</v>
       </c>
+      <c r="W11" s="5">
+        <f t="shared" si="2"/>
+        <v>536</v>
+      </c>
+      <c r="X11" s="6">
+        <f t="shared" si="3"/>
+        <v>367</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="4"/>
+        <v>381</v>
+      </c>
+      <c r="Z11" s="6">
+        <f t="shared" si="5"/>
+        <v>401</v>
+      </c>
+      <c r="AA11" s="6">
+        <f t="shared" si="6"/>
+        <v>461</v>
+      </c>
+      <c r="AB11" s="6">
+        <f t="shared" si="7"/>
+        <v>521</v>
+      </c>
+      <c r="AC11" s="6">
+        <f t="shared" si="8"/>
+        <v>492</v>
+      </c>
+      <c r="AD11" s="6">
+        <f t="shared" si="9"/>
+        <v>562</v>
+      </c>
+      <c r="AE11" s="6">
+        <f t="shared" si="10"/>
+        <v>517</v>
+      </c>
+      <c r="AF11" s="6">
+        <f t="shared" si="11"/>
+        <v>616</v>
+      </c>
+      <c r="AG11" s="6">
+        <f t="shared" si="12"/>
+        <v>637</v>
+      </c>
+      <c r="AH11" s="6">
+        <f t="shared" si="13"/>
+        <v>694</v>
+      </c>
+      <c r="AI11" s="6">
+        <f t="shared" si="14"/>
+        <v>697</v>
+      </c>
+      <c r="AJ11" s="6">
+        <f t="shared" si="15"/>
+        <v>707</v>
+      </c>
+      <c r="AK11" s="6">
+        <f t="shared" si="21"/>
+        <v>787</v>
+      </c>
+      <c r="AL11">
+        <f t="shared" si="16"/>
+        <v>815</v>
+      </c>
+      <c r="AM11" s="6">
+        <f t="shared" si="17"/>
+        <v>864</v>
+      </c>
+      <c r="AN11" s="6">
+        <f t="shared" si="18"/>
+        <v>929</v>
+      </c>
+      <c r="AO11" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP11" s="7">
+        <f t="shared" si="20"/>
+        <v>949</v>
+      </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>8</v>
       </c>
@@ -1169,8 +1952,86 @@
       <c r="U12" s="7">
         <v>12</v>
       </c>
+      <c r="W12" s="5">
+        <f t="shared" si="2"/>
+        <v>544</v>
+      </c>
+      <c r="X12" s="6">
+        <f t="shared" si="3"/>
+        <v>370</v>
+      </c>
+      <c r="Y12" s="6">
+        <f t="shared" si="4"/>
+        <v>447</v>
+      </c>
+      <c r="Z12" s="6">
+        <f t="shared" si="5"/>
+        <v>431</v>
+      </c>
+      <c r="AA12" s="6">
+        <f t="shared" si="6"/>
+        <v>462</v>
+      </c>
+      <c r="AB12" s="6">
+        <f t="shared" si="7"/>
+        <v>484</v>
+      </c>
+      <c r="AC12" s="6">
+        <f t="shared" si="8"/>
+        <v>511</v>
+      </c>
+      <c r="AD12" s="6">
+        <f t="shared" si="9"/>
+        <v>564</v>
+      </c>
+      <c r="AE12" s="6">
+        <f t="shared" si="10"/>
+        <v>580</v>
+      </c>
+      <c r="AF12" s="6">
+        <f t="shared" si="11"/>
+        <v>670</v>
+      </c>
+      <c r="AG12" s="6">
+        <f t="shared" si="12"/>
+        <v>708</v>
+      </c>
+      <c r="AH12" s="6">
+        <f t="shared" si="13"/>
+        <v>758</v>
+      </c>
+      <c r="AI12" s="6">
+        <f t="shared" si="14"/>
+        <v>788</v>
+      </c>
+      <c r="AJ12" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK12" s="6">
+        <f t="shared" si="21"/>
+        <v>792</v>
+      </c>
+      <c r="AL12" s="6">
+        <f t="shared" si="16"/>
+        <v>821</v>
+      </c>
+      <c r="AM12" s="6">
+        <f t="shared" si="17"/>
+        <v>913</v>
+      </c>
+      <c r="AN12" s="6">
+        <f t="shared" si="18"/>
+        <v>1000</v>
+      </c>
+      <c r="AO12" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP12" s="7">
+        <f t="shared" si="20"/>
+        <v>961</v>
+      </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>70</v>
       </c>
@@ -1231,8 +2092,83 @@
       <c r="U13" s="7">
         <v>13</v>
       </c>
+      <c r="W13" s="5">
+        <f t="shared" si="2"/>
+        <v>614</v>
+      </c>
+      <c r="X13" s="6">
+        <f t="shared" si="3"/>
+        <v>409</v>
+      </c>
+      <c r="Y13" s="6">
+        <f t="shared" si="4"/>
+        <v>491</v>
+      </c>
+      <c r="Z13" s="6">
+        <f t="shared" si="5"/>
+        <v>492</v>
+      </c>
+      <c r="AA13" s="6">
+        <f t="shared" si="6"/>
+        <v>515</v>
+      </c>
+      <c r="AB13" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AC13" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AD13" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AE13" s="6">
+        <f t="shared" si="10"/>
+        <v>593</v>
+      </c>
+      <c r="AF13" s="6">
+        <f t="shared" si="11"/>
+        <v>629</v>
+      </c>
+      <c r="AG13" s="6">
+        <f t="shared" si="12"/>
+        <v>699</v>
+      </c>
+      <c r="AH13" s="6">
+        <f t="shared" si="13"/>
+        <v>714</v>
+      </c>
+      <c r="AI13" s="6">
+        <f t="shared" si="14"/>
+        <v>750</v>
+      </c>
+      <c r="AJ13" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK13" s="6">
+        <f t="shared" si="21"/>
+        <v>884</v>
+      </c>
+      <c r="AL13" s="6">
+        <f t="shared" si="16"/>
+        <v>874</v>
+      </c>
+      <c r="AM13" s="6">
+        <f t="shared" si="17"/>
+        <v>881</v>
+      </c>
+      <c r="AN13" s="6">
+        <f t="shared" si="18"/>
+        <v>895</v>
+      </c>
+      <c r="AO13" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP13" s="7">
+        <f t="shared" si="20"/>
+        <v>974</v>
+      </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>96</v>
       </c>
@@ -1293,8 +2229,85 @@
       <c r="U14" s="7">
         <v>77</v>
       </c>
+      <c r="W14" s="5">
+        <f t="shared" si="2"/>
+        <v>710</v>
+      </c>
+      <c r="X14" s="6">
+        <f t="shared" si="3"/>
+        <v>458</v>
+      </c>
+      <c r="Y14" s="6">
+        <f t="shared" si="4"/>
+        <v>535</v>
+      </c>
+      <c r="Z14" s="6">
+        <f t="shared" si="5"/>
+        <v>510</v>
+      </c>
+      <c r="AA14" s="6">
+        <f t="shared" si="6"/>
+        <v>575</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="7"/>
+        <v>666</v>
+      </c>
+      <c r="AC14" s="6">
+        <f t="shared" si="8"/>
+        <v>682</v>
+      </c>
+      <c r="AD14" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AE14" s="6">
+        <f t="shared" si="10"/>
+        <v>683</v>
+      </c>
+      <c r="AF14" s="6">
+        <f t="shared" si="11"/>
+        <v>707</v>
+      </c>
+      <c r="AG14" s="6">
+        <f t="shared" si="12"/>
+        <v>719</v>
+      </c>
+      <c r="AH14" s="6">
+        <f t="shared" si="13"/>
+        <v>789</v>
+      </c>
+      <c r="AI14" s="6">
+        <f t="shared" si="14"/>
+        <v>764</v>
+      </c>
+      <c r="AJ14" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK14" s="6">
+        <f t="shared" si="21"/>
+        <v>913</v>
+      </c>
+      <c r="AL14" s="6">
+        <f t="shared" si="16"/>
+        <v>923</v>
+      </c>
+      <c r="AM14" s="6">
+        <f t="shared" si="17"/>
+        <v>945</v>
+      </c>
+      <c r="AN14" s="6">
+        <f t="shared" si="18"/>
+        <v>966</v>
+      </c>
+      <c r="AO14" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP14" s="7">
+        <f t="shared" si="20"/>
+        <v>1051</v>
+      </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>73</v>
       </c>
@@ -1355,8 +2368,85 @@
       <c r="U15" s="7">
         <v>42</v>
       </c>
+      <c r="W15" s="5">
+        <f t="shared" si="2"/>
+        <v>783</v>
+      </c>
+      <c r="X15" s="6">
+        <f t="shared" si="3"/>
+        <v>464</v>
+      </c>
+      <c r="Y15" s="6">
+        <f t="shared" si="4"/>
+        <v>542</v>
+      </c>
+      <c r="Z15" s="6">
+        <f t="shared" si="5"/>
+        <v>582</v>
+      </c>
+      <c r="AA15" s="6">
+        <f t="shared" si="6"/>
+        <v>588</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="7"/>
+        <v>619</v>
+      </c>
+      <c r="AC15" s="6">
+        <f t="shared" si="8"/>
+        <v>623</v>
+      </c>
+      <c r="AD15" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AE15" s="6">
+        <f t="shared" si="10"/>
+        <v>712</v>
+      </c>
+      <c r="AF15" s="6">
+        <f t="shared" si="11"/>
+        <v>750</v>
+      </c>
+      <c r="AG15" s="6">
+        <f t="shared" si="12"/>
+        <v>766</v>
+      </c>
+      <c r="AH15" s="6">
+        <f t="shared" si="13"/>
+        <v>813</v>
+      </c>
+      <c r="AI15" s="6">
+        <f t="shared" si="14"/>
+        <v>844</v>
+      </c>
+      <c r="AJ15" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK15" s="6">
+        <f t="shared" si="21"/>
+        <v>940</v>
+      </c>
+      <c r="AL15" s="6">
+        <f t="shared" si="16"/>
+        <v>969</v>
+      </c>
+      <c r="AM15" s="6">
+        <f t="shared" si="17"/>
+        <v>973</v>
+      </c>
+      <c r="AN15" s="6">
+        <f t="shared" si="18"/>
+        <v>1063</v>
+      </c>
+      <c r="AO15" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AP15" s="7">
+        <f t="shared" si="20"/>
+        <v>1093</v>
+      </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>21</v>
       </c>
@@ -1417,8 +2507,86 @@
       <c r="U16" s="7">
         <v>25</v>
       </c>
+      <c r="W16" s="5">
+        <f t="shared" si="2"/>
+        <v>804</v>
+      </c>
+      <c r="X16" s="6">
+        <f t="shared" si="3"/>
+        <v>472</v>
+      </c>
+      <c r="Y16" s="6">
+        <f t="shared" si="4"/>
+        <v>559</v>
+      </c>
+      <c r="Z16" s="6">
+        <f t="shared" si="5"/>
+        <v>584</v>
+      </c>
+      <c r="AA16" s="6">
+        <f t="shared" si="6"/>
+        <v>622</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="7"/>
+        <v>693</v>
+      </c>
+      <c r="AC16" s="6">
+        <f t="shared" si="8"/>
+        <v>662</v>
+      </c>
+      <c r="AD16" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AE16" s="6">
+        <f t="shared" si="10"/>
+        <v>729</v>
+      </c>
+      <c r="AF16" s="6">
+        <f t="shared" si="11"/>
+        <v>740</v>
+      </c>
+      <c r="AG16" s="6">
+        <f t="shared" si="12"/>
+        <v>747</v>
+      </c>
+      <c r="AH16" s="6">
+        <f t="shared" si="13"/>
+        <v>765</v>
+      </c>
+      <c r="AI16" s="6">
+        <f t="shared" si="14"/>
+        <v>857</v>
+      </c>
+      <c r="AJ16" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK16" s="6">
+        <f t="shared" si="21"/>
+        <v>978</v>
+      </c>
+      <c r="AL16" s="6">
+        <f t="shared" si="16"/>
+        <v>993</v>
+      </c>
+      <c r="AM16" s="6">
+        <f t="shared" si="17"/>
+        <v>1071</v>
+      </c>
+      <c r="AN16" s="6">
+        <f t="shared" si="18"/>
+        <v>1115</v>
+      </c>
+      <c r="AO16" s="6">
+        <f t="shared" si="19"/>
+        <v>1162</v>
+      </c>
+      <c r="AP16" s="7">
+        <f t="shared" si="20"/>
+        <v>1118</v>
+      </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>12</v>
       </c>
@@ -1479,8 +2647,86 @@
       <c r="U17" s="9">
         <v>23</v>
       </c>
+      <c r="W17" s="5">
+        <f t="shared" si="2"/>
+        <v>816</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="3"/>
+        <v>517</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="4"/>
+        <v>575</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="5"/>
+        <v>662</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="6"/>
+        <v>676</v>
+      </c>
+      <c r="AB17" s="6">
+        <f t="shared" si="7"/>
+        <v>750</v>
+      </c>
+      <c r="AC17" s="6">
+        <f t="shared" si="8"/>
+        <v>739</v>
+      </c>
+      <c r="AD17" s="13">
+        <v>100000</v>
+      </c>
+      <c r="AE17" s="6">
+        <f t="shared" si="10"/>
+        <v>783</v>
+      </c>
+      <c r="AF17" s="6">
+        <f t="shared" si="11"/>
+        <v>833</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="12"/>
+        <v>756</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="13"/>
+        <v>811</v>
+      </c>
+      <c r="AI17" s="15">
+        <f t="shared" si="14"/>
+        <v>850</v>
+      </c>
+      <c r="AJ17" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK17" s="6">
+        <f t="shared" si="21"/>
+        <v>1044</v>
+      </c>
+      <c r="AL17" s="6">
+        <f t="shared" si="16"/>
+        <v>1032</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="17"/>
+        <v>1130</v>
+      </c>
+      <c r="AN17" s="6">
+        <f t="shared" si="18"/>
+        <v>1148</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="19"/>
+        <v>1198</v>
+      </c>
+      <c r="AP17" s="9">
+        <f t="shared" si="20"/>
+        <v>1141</v>
+      </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>51</v>
       </c>
@@ -1541,8 +2787,84 @@
       <c r="U18" s="9">
         <v>65</v>
       </c>
+      <c r="W18" s="5">
+        <f t="shared" si="2"/>
+        <v>867</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="3"/>
+        <v>530</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="4"/>
+        <v>624</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="5"/>
+        <v>655</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="6"/>
+        <v>678</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="7"/>
+        <v>683</v>
+      </c>
+      <c r="AC18" s="6">
+        <f t="shared" si="8"/>
+        <v>707</v>
+      </c>
+      <c r="AD18" s="6">
+        <f t="shared" si="9"/>
+        <v>721</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="10"/>
+        <v>795</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="11"/>
+        <v>885</v>
+      </c>
+      <c r="AG18" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AH18" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AI18" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AJ18" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="AK18" s="6">
+        <f t="shared" si="21"/>
+        <v>1074</v>
+      </c>
+      <c r="AL18" s="6">
+        <f t="shared" si="16"/>
+        <v>1131</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="17"/>
+        <v>1139</v>
+      </c>
+      <c r="AN18" s="6">
+        <f t="shared" si="18"/>
+        <v>1232</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="19"/>
+        <v>1260</v>
+      </c>
+      <c r="AP18" s="9">
+        <f t="shared" si="20"/>
+        <v>1206</v>
+      </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>76</v>
       </c>
@@ -1603,8 +2925,88 @@
       <c r="U19" s="9">
         <v>76</v>
       </c>
+      <c r="W19" s="5">
+        <f t="shared" si="2"/>
+        <v>943</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="3"/>
+        <v>545</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="4"/>
+        <v>644</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="5"/>
+        <v>709</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="6"/>
+        <v>745</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="7"/>
+        <v>743</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="8"/>
+        <v>799</v>
+      </c>
+      <c r="AD19" s="6">
+        <f t="shared" si="9"/>
+        <v>736</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="10"/>
+        <v>830</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="11"/>
+        <v>846</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="12"/>
+        <v>902</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="13"/>
+        <v>971</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" si="14"/>
+        <v>1069</v>
+      </c>
+      <c r="AJ19">
+        <f t="shared" si="15"/>
+        <v>1151</v>
+      </c>
+      <c r="AK19">
+        <f t="shared" si="21"/>
+        <v>1146</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" si="16"/>
+        <v>1170</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="17"/>
+        <v>1207</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="18"/>
+        <v>1225</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="19"/>
+        <v>1278</v>
+      </c>
+      <c r="AP19" s="9">
+        <f t="shared" si="20"/>
+        <v>1282</v>
+      </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>87</v>
       </c>
@@ -1665,8 +3067,88 @@
       <c r="U20" s="9">
         <v>4</v>
       </c>
+      <c r="W20" s="5">
+        <f t="shared" si="2"/>
+        <v>1030</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="3"/>
+        <v>593</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="4"/>
+        <v>683</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="5"/>
+        <v>739</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="6"/>
+        <v>779</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="7"/>
+        <v>834</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="8"/>
+        <v>860</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="9"/>
+        <v>747</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="10"/>
+        <v>749</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="11"/>
+        <v>835</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="12"/>
+        <v>859</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="13"/>
+        <v>936</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="14"/>
+        <v>953</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" si="15"/>
+        <v>1042</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" si="21"/>
+        <v>1110</v>
+      </c>
+      <c r="AL20">
+        <f t="shared" si="16"/>
+        <v>1144</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="17"/>
+        <v>1155</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="18"/>
+        <v>1238</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="19"/>
+        <v>1326</v>
+      </c>
+      <c r="AP20" s="9">
+        <f t="shared" si="20"/>
+        <v>1286</v>
+      </c>
     </row>
-    <row r="21" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>43</v>
       </c>
@@ -1726,6 +3208,94 @@
       </c>
       <c r="U21" s="12">
         <v>53</v>
+      </c>
+      <c r="W21" s="5">
+        <f t="shared" si="2"/>
+        <v>1073</v>
+      </c>
+      <c r="X21" s="11">
+        <f t="shared" si="3"/>
+        <v>681</v>
+      </c>
+      <c r="Y21" s="11">
+        <f t="shared" si="4"/>
+        <v>710</v>
+      </c>
+      <c r="Z21" s="11">
+        <f t="shared" si="5"/>
+        <v>751</v>
+      </c>
+      <c r="AA21" s="11">
+        <f t="shared" si="6"/>
+        <v>757</v>
+      </c>
+      <c r="AB21" s="11">
+        <f t="shared" si="7"/>
+        <v>796</v>
+      </c>
+      <c r="AC21" s="11">
+        <f t="shared" si="8"/>
+        <v>887</v>
+      </c>
+      <c r="AD21" s="11">
+        <f t="shared" si="9"/>
+        <v>794</v>
+      </c>
+      <c r="AE21" s="11">
+        <f t="shared" si="10"/>
+        <v>787</v>
+      </c>
+      <c r="AF21" s="11">
+        <f t="shared" si="11"/>
+        <v>810</v>
+      </c>
+      <c r="AG21" s="11">
+        <f t="shared" si="12"/>
+        <v>854</v>
+      </c>
+      <c r="AH21" s="11">
+        <f t="shared" si="13"/>
+        <v>873</v>
+      </c>
+      <c r="AI21" s="11">
+        <f t="shared" si="14"/>
+        <v>947</v>
+      </c>
+      <c r="AJ21" s="11">
+        <f t="shared" si="15"/>
+        <v>980</v>
+      </c>
+      <c r="AK21" s="11">
+        <f t="shared" si="21"/>
+        <v>1011</v>
+      </c>
+      <c r="AL21" s="11">
+        <f t="shared" si="16"/>
+        <v>1029</v>
+      </c>
+      <c r="AM21" s="11">
+        <f t="shared" si="17"/>
+        <v>1055</v>
+      </c>
+      <c r="AN21" s="11">
+        <f t="shared" si="18"/>
+        <v>1103</v>
+      </c>
+      <c r="AO21" s="11">
+        <f t="shared" si="19"/>
+        <v>1200</v>
+      </c>
+      <c r="AP21" s="14">
+        <f t="shared" si="20"/>
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="25" spans="2:42" x14ac:dyDescent="0.25">
+      <c r="Y25" s="17">
+        <v>1253</v>
+      </c>
+      <c r="Z25">
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>